<commit_message>
1st day heat map (1 response missing) + used csv
</commit_message>
<xml_diff>
--- a/heatmaps/R-scr/HM-MS2.xlsx
+++ b/heatmaps/R-scr/HM-MS2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25605" windowHeight="15480" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11700" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Codes" sheetId="9" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Day-4" sheetId="7" r:id="rId5"/>
     <sheet name="Day-5" sheetId="8" r:id="rId6"/>
     <sheet name="Average" sheetId="5" r:id="rId7"/>
+    <sheet name="HM Names" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="133">
   <si>
     <t>PgM</t>
   </si>
@@ -223,6 +224,219 @@
   </si>
   <si>
     <t>N-XFT-5</t>
+  </si>
+  <si>
+    <t>HM Name</t>
+  </si>
+  <si>
+    <t>Daniel Fr</t>
+  </si>
+  <si>
+    <t>Henrik</t>
+  </si>
+  <si>
+    <t>Helena</t>
+  </si>
+  <si>
+    <t>Nihal</t>
+  </si>
+  <si>
+    <t>Magnus</t>
+  </si>
+  <si>
+    <t>Xi</t>
+  </si>
+  <si>
+    <t>Joakim</t>
+  </si>
+  <si>
+    <t>Jonas</t>
+  </si>
+  <si>
+    <t>Anders</t>
+  </si>
+  <si>
+    <t>Johan</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>O1-I</t>
+  </si>
+  <si>
+    <t>O1-N</t>
+  </si>
+  <si>
+    <t>O (Administrative)</t>
+  </si>
+  <si>
+    <t>Lars Johansson</t>
+  </si>
+  <si>
+    <t>O1</t>
+  </si>
+  <si>
+    <t>O2-I</t>
+  </si>
+  <si>
+    <t>O2-N</t>
+  </si>
+  <si>
+    <t>O2</t>
+  </si>
+  <si>
+    <t>Anna Lanner</t>
+  </si>
+  <si>
+    <t>Lena Serra</t>
+  </si>
+  <si>
+    <t>CEB-adm.</t>
+  </si>
+  <si>
+    <t>O3</t>
+  </si>
+  <si>
+    <t>O3-I</t>
+  </si>
+  <si>
+    <t>O3-N</t>
+  </si>
+  <si>
+    <t>O4-I</t>
+  </si>
+  <si>
+    <t>O4-N</t>
+  </si>
+  <si>
+    <t>Main TC</t>
+  </si>
+  <si>
+    <t>O4</t>
+  </si>
+  <si>
+    <t>Design (MS3)</t>
+  </si>
+  <si>
+    <t>Magnus Bergh</t>
+  </si>
+  <si>
+    <t>OPO2</t>
+  </si>
+  <si>
+    <t>OPO2-I</t>
+  </si>
+  <si>
+    <t>OPO2-N</t>
+  </si>
+  <si>
+    <t>O (Planning data future sprints</t>
+  </si>
+  <si>
+    <t>APO</t>
+  </si>
+  <si>
+    <t>APO1</t>
+  </si>
+  <si>
+    <t>Björn Ternström</t>
+  </si>
+  <si>
+    <t>Elizabeth Hansson</t>
+  </si>
+  <si>
+    <t>CA Kanban Master</t>
+  </si>
+  <si>
+    <t>O5</t>
+  </si>
+  <si>
+    <t>O5-I</t>
+  </si>
+  <si>
+    <t>O5-N</t>
+  </si>
+  <si>
+    <t>Future planning next release</t>
+  </si>
+  <si>
+    <t>APO1-I</t>
+  </si>
+  <si>
+    <t>APO1-N</t>
+  </si>
+  <si>
+    <t>Marcel van Torgeren</t>
+  </si>
+  <si>
+    <t>PgM2</t>
+  </si>
+  <si>
+    <t>PgM2-I</t>
+  </si>
+  <si>
+    <t>PgM2-N</t>
+  </si>
+  <si>
+    <t>O (P5G preparation)</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>Helena Ebnil</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>O6</t>
+  </si>
+  <si>
+    <t>O6-I</t>
+  </si>
+  <si>
+    <t>O6-N</t>
+  </si>
+  <si>
+    <t>Simeon Soetan</t>
+  </si>
+  <si>
+    <t>Designer</t>
+  </si>
+  <si>
+    <t>O7</t>
+  </si>
+  <si>
+    <t>O7-I</t>
+  </si>
+  <si>
+    <t>O7-N</t>
+  </si>
+  <si>
+    <t>Marja Hammarstrand</t>
+  </si>
+  <si>
+    <t>OPO3</t>
+  </si>
+  <si>
+    <t>Marcus Larsson</t>
+  </si>
+  <si>
+    <t>OPO3-I</t>
+  </si>
+  <si>
+    <t>OPO3-N</t>
   </si>
 </sst>
 </file>
@@ -280,7 +494,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -299,8 +513,20 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -336,6 +562,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -362,7 +599,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -381,6 +618,18 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -739,15 +988,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -869,6 +1119,124 @@
       </c>
       <c r="C11" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" t="s">
+        <v>93</v>
+      </c>
+      <c r="C16" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>96</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>103</v>
+      </c>
+      <c r="B18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B20" t="s">
+        <v>0</v>
+      </c>
+      <c r="C20" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>118</v>
+      </c>
+      <c r="B21" t="s">
+        <v>119</v>
+      </c>
+      <c r="C21" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22" t="s">
+        <v>124</v>
+      </c>
+      <c r="C22" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>130</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -879,18 +1247,60 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W12"/>
+  <dimension ref="A1:AS12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:W1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="23" width="6.125" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="3.125" customWidth="1"/>
+    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="5" max="5" width="4.125" customWidth="1"/>
+    <col min="6" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="3.375" customWidth="1"/>
+    <col min="8" max="8" width="7" customWidth="1"/>
+    <col min="9" max="9" width="3.375" customWidth="1"/>
+    <col min="10" max="10" width="7" customWidth="1"/>
+    <col min="11" max="11" width="3.625" customWidth="1"/>
+    <col min="12" max="12" width="7" customWidth="1"/>
+    <col min="13" max="13" width="3.375" customWidth="1"/>
+    <col min="14" max="14" width="7" customWidth="1"/>
+    <col min="15" max="15" width="3" customWidth="1"/>
+    <col min="16" max="16" width="7" customWidth="1"/>
+    <col min="17" max="17" width="3.125" customWidth="1"/>
+    <col min="18" max="18" width="7" customWidth="1"/>
+    <col min="19" max="19" width="2.875" customWidth="1"/>
+    <col min="20" max="20" width="7" customWidth="1"/>
+    <col min="21" max="21" width="2.75" customWidth="1"/>
+    <col min="22" max="22" width="7" customWidth="1"/>
+    <col min="23" max="23" width="3.25" customWidth="1"/>
+    <col min="24" max="24" width="8" customWidth="1"/>
+    <col min="25" max="25" width="5.125" customWidth="1"/>
+    <col min="26" max="26" width="6.375" customWidth="1"/>
+    <col min="27" max="27" width="6.125" customWidth="1"/>
+    <col min="28" max="28" width="6.5" customWidth="1"/>
+    <col min="29" max="29" width="3.75" customWidth="1"/>
+    <col min="30" max="30" width="6.75" customWidth="1"/>
+    <col min="31" max="31" width="6" customWidth="1"/>
+    <col min="32" max="32" width="6.75" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="4.875" customWidth="1"/>
+    <col min="34" max="34" width="4.75" customWidth="1"/>
+    <col min="35" max="35" width="6" customWidth="1"/>
+    <col min="36" max="37" width="6.75" customWidth="1"/>
+    <col min="38" max="38" width="7.5" customWidth="1"/>
+    <col min="39" max="39" width="8.75" customWidth="1"/>
+    <col min="40" max="40" width="6.625" customWidth="1"/>
+    <col min="41" max="41" width="5.5" customWidth="1"/>
+    <col min="42" max="42" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="5.125" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="6.875" customWidth="1"/>
+    <col min="45" max="45" width="4.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>6</v>
@@ -916,10 +1326,10 @@
       <c r="I1" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="K1" s="16" t="s">
         <v>59</v>
       </c>
       <c r="L1" s="4" t="s">
@@ -958,83 +1368,411 @@
       <c r="W1" s="5" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X1" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y1" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z1" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="AA1" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="AB1" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="AD1" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="AE1" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="AF1" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="AG1" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="AH1" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="AI1" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ1" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="AK1" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="AL1" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="AM1" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="AN1" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="AO1" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="AR1" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="AS1" s="13" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F2" s="17">
+        <v>3</v>
+      </c>
+      <c r="G2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H2" s="17">
+        <v>3</v>
+      </c>
+      <c r="I2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2">
+        <v>3</v>
+      </c>
+      <c r="M2" t="s">
+        <v>73</v>
+      </c>
+      <c r="P2">
+        <v>3</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>74</v>
+      </c>
+      <c r="T2">
+        <v>5</v>
+      </c>
+      <c r="U2" t="s">
+        <v>79</v>
+      </c>
+      <c r="X2" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>73</v>
+      </c>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
+      <c r="L3">
+        <v>3</v>
+      </c>
+      <c r="M3" t="s">
+        <v>73</v>
+      </c>
+      <c r="X3" s="17">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
+      <c r="AB4" s="17">
+        <v>2</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD4" s="17">
+        <v>2</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5">
+        <v>4</v>
+      </c>
+      <c r="G5" t="s">
+        <v>117</v>
+      </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5">
+        <v>3</v>
+      </c>
+      <c r="M5" t="s">
+        <v>117</v>
+      </c>
+      <c r="X5" s="17">
+        <v>4</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>117</v>
+      </c>
+      <c r="AN5" s="17">
+        <v>4</v>
+      </c>
+      <c r="AO5" t="s">
+        <v>74</v>
+      </c>
+      <c r="AP5">
+        <v>4</v>
+      </c>
+      <c r="AQ5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15"/>
+      <c r="V6" s="15"/>
+      <c r="W6" s="15"/>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>75</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
       <c r="L7" s="2"/>
       <c r="M7" s="2"/>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="N7" s="17">
+        <v>2</v>
+      </c>
+      <c r="O7" t="s">
+        <v>75</v>
+      </c>
+      <c r="X7">
+        <v>1</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8">
+        <v>2</v>
+      </c>
+      <c r="M8" t="s">
+        <v>76</v>
+      </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="P8">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>74</v>
+      </c>
+      <c r="AF8">
+        <v>2</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B9" s="17">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="N9" s="17">
+        <v>2</v>
+      </c>
+      <c r="O9" t="s">
+        <v>76</v>
+      </c>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="V9">
+        <v>1</v>
+      </c>
+      <c r="AR9">
+        <v>6</v>
+      </c>
+      <c r="AS9" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="P12">
+        <v>2</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>100</v>
+      </c>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
+      <c r="AD12">
+        <v>3</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AH12">
+        <v>3</v>
+      </c>
+      <c r="AI12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AJ12">
+        <v>3</v>
+      </c>
+      <c r="AK12" t="s">
+        <v>109</v>
+      </c>
+      <c r="AL12">
+        <v>3</v>
+      </c>
+      <c r="AM12" t="s">
+        <v>116</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1052,7 +1790,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1442,7 +2180,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:W1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1831,7 +2569,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W1" sqref="B1:W1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2220,7 +2958,7 @@
   <dimension ref="A1:W12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2608,8 +3346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3354,4 +4092,152 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Includes final data for day 1
</commit_message>
<xml_diff>
--- a/heatmaps/R-scr/HM-MS2.xlsx
+++ b/heatmaps/R-scr/HM-MS2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="150">
   <si>
     <t>PgM</t>
   </si>
@@ -437,6 +437,57 @@
   </si>
   <si>
     <t>OPO3-N</t>
+  </si>
+  <si>
+    <t>Henric Stenhoff</t>
+  </si>
+  <si>
+    <t>DM</t>
+  </si>
+  <si>
+    <t>DM2</t>
+  </si>
+  <si>
+    <t>Patrik Främme</t>
+  </si>
+  <si>
+    <t>SM</t>
+  </si>
+  <si>
+    <t>SM2</t>
+  </si>
+  <si>
+    <t>Björn Östlund</t>
+  </si>
+  <si>
+    <t>TM Manager</t>
+  </si>
+  <si>
+    <t>TM1</t>
+  </si>
+  <si>
+    <t>DM2-I</t>
+  </si>
+  <si>
+    <t>DM2-N</t>
+  </si>
+  <si>
+    <t>SM2-I</t>
+  </si>
+  <si>
+    <t>SM2-N</t>
+  </si>
+  <si>
+    <t>TM1-I</t>
+  </si>
+  <si>
+    <t>TM1-N</t>
+  </si>
+  <si>
+    <t>Recruitment</t>
+  </si>
+  <si>
+    <t>Sector Goals</t>
   </si>
 </sst>
 </file>
@@ -988,10 +1039,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1239,6 +1290,39 @@
         <v>129</v>
       </c>
     </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>133</v>
+      </c>
+      <c r="B24" t="s">
+        <v>134</v>
+      </c>
+      <c r="C24" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>136</v>
+      </c>
+      <c r="B25" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>139</v>
+      </c>
+      <c r="B26" t="s">
+        <v>140</v>
+      </c>
+      <c r="C26" t="s">
+        <v>141</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1247,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS12"/>
+  <dimension ref="A1:AY12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="AX11" sqref="AX11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1298,9 +1382,15 @@
     <col min="43" max="43" width="5.125" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="6.875" customWidth="1"/>
     <col min="45" max="45" width="4.5" customWidth="1"/>
+    <col min="46" max="46" width="6.375" customWidth="1"/>
+    <col min="47" max="47" width="4.125" customWidth="1"/>
+    <col min="48" max="48" width="7.25" customWidth="1"/>
+    <col min="49" max="49" width="4.625" customWidth="1"/>
+    <col min="50" max="50" width="7.75" customWidth="1"/>
+    <col min="51" max="51" width="4.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="3" t="s">
         <v>6</v>
@@ -1434,8 +1524,26 @@
       <c r="AS1" s="13" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT1" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="AU1" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="AV1" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="AW1" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="AX1" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="AY1" s="13" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1492,7 +1600,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
@@ -1519,7 +1627,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
@@ -1540,7 +1648,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>49</v>
       </c>
@@ -1585,7 +1693,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>50</v>
       </c>
@@ -1612,7 +1720,7 @@
       <c r="V6" s="15"/>
       <c r="W6" s="15"/>
     </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>51</v>
       </c>
@@ -1651,7 +1759,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>2</v>
       </c>
@@ -1681,7 +1789,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>3</v>
       </c>
@@ -1717,7 +1825,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>4</v>
       </c>
@@ -1726,7 +1834,7 @@
       <c r="R10" s="2"/>
       <c r="S10" s="2"/>
     </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>5</v>
       </c>
@@ -1734,8 +1842,26 @@
       <c r="K11" s="15"/>
       <c r="T11" s="2"/>
       <c r="U11" s="2"/>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="AT11" s="17">
+        <v>5</v>
+      </c>
+      <c r="AU11" t="s">
+        <v>148</v>
+      </c>
+      <c r="AV11" s="17">
+        <v>4</v>
+      </c>
+      <c r="AW11" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX11" s="17">
+        <v>2</v>
+      </c>
+      <c r="AY11" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="12" spans="1:51" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Includes updated ids and new others
</commit_message>
<xml_diff>
--- a/heatmaps/R-scr/HM-MS2.xlsx
+++ b/heatmaps/R-scr/HM-MS2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11700" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="20730" windowHeight="11700" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Codes" sheetId="9" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="194">
   <si>
     <t>PgM</t>
   </si>
@@ -283,9 +283,6 @@
     <t>Lars Johansson</t>
   </si>
   <si>
-    <t>O1</t>
-  </si>
-  <si>
     <t>O2-I</t>
   </si>
   <si>
@@ -301,12 +298,6 @@
     <t>Lena Serra</t>
   </si>
   <si>
-    <t>CEB-adm.</t>
-  </si>
-  <si>
-    <t>O3</t>
-  </si>
-  <si>
     <t>O3-I</t>
   </si>
   <si>
@@ -322,9 +313,6 @@
     <t>Main TC</t>
   </si>
   <si>
-    <t>O4</t>
-  </si>
-  <si>
     <t>Design (MS3)</t>
   </si>
   <si>
@@ -358,9 +346,6 @@
     <t>CA Kanban Master</t>
   </si>
   <si>
-    <t>O5</t>
-  </si>
-  <si>
     <t>O5-I</t>
   </si>
   <si>
@@ -394,9 +379,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>Helena Ebnil</t>
-  </si>
-  <si>
     <t>Manager</t>
   </si>
   <si>
@@ -488,6 +470,156 @@
   </si>
   <si>
     <t>Sector Goals</t>
+  </si>
+  <si>
+    <t>Survey Code</t>
+  </si>
+  <si>
+    <t>PgM1</t>
+  </si>
+  <si>
+    <t>CAKM1</t>
+  </si>
+  <si>
+    <t>XFT-SM1</t>
+  </si>
+  <si>
+    <t>Dsgnr1</t>
+  </si>
+  <si>
+    <t>Dsgnr2</t>
+  </si>
+  <si>
+    <t>Lars Rundberg</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Dsgnr3</t>
+  </si>
+  <si>
+    <t>Eva Cullman</t>
+  </si>
+  <si>
+    <t>Mikael Krekola</t>
+  </si>
+  <si>
+    <t>PG-froCpp</t>
+  </si>
+  <si>
+    <t>XFT-PG1</t>
+  </si>
+  <si>
+    <t>PG3</t>
+  </si>
+  <si>
+    <t>Pierre Svärd</t>
+  </si>
+  <si>
+    <t>Dsgnr4</t>
+  </si>
+  <si>
+    <t>TC1</t>
+  </si>
+  <si>
+    <t>CCB-A</t>
+  </si>
+  <si>
+    <t>CCB-adm.</t>
+  </si>
+  <si>
+    <t>Anny Lei</t>
+  </si>
+  <si>
+    <t>Feature Proj. Leader</t>
+  </si>
+  <si>
+    <t>FPjL1</t>
+  </si>
+  <si>
+    <t>Jan Johansson</t>
+  </si>
+  <si>
+    <t>Prod. Manager RBS Sys</t>
+  </si>
+  <si>
+    <t>PdMRBS1</t>
+  </si>
+  <si>
+    <t>Per Simonsson</t>
+  </si>
+  <si>
+    <t>RBS System</t>
+  </si>
+  <si>
+    <t>RBS1</t>
+  </si>
+  <si>
+    <t>Henrik Sundh</t>
+  </si>
+  <si>
+    <t>Strategic Product Manager</t>
+  </si>
+  <si>
+    <t>SPM1</t>
+  </si>
+  <si>
+    <t>Helena Eberil</t>
+  </si>
+  <si>
+    <t>Jeanette Munro</t>
+  </si>
+  <si>
+    <t>Dsgnr5</t>
+  </si>
+  <si>
+    <t>Ricardo Morales</t>
+  </si>
+  <si>
+    <t>Dsgnr6</t>
+  </si>
+  <si>
+    <t>Carl Ohlsson</t>
+  </si>
+  <si>
+    <t>Dsgnr7</t>
+  </si>
+  <si>
+    <t>PgM3</t>
+  </si>
+  <si>
+    <t>Niklas Isaksson</t>
+  </si>
+  <si>
+    <t>Program Manager</t>
+  </si>
+  <si>
+    <t>Thomas Andersson</t>
+  </si>
+  <si>
+    <t>Sector Manager</t>
+  </si>
+  <si>
+    <t>SrM1</t>
+  </si>
+  <si>
+    <t>Per Lofter</t>
+  </si>
+  <si>
+    <t>Section Manager</t>
+  </si>
+  <si>
+    <t>SM3</t>
+  </si>
+  <si>
+    <t>Thomas Nyberg</t>
+  </si>
+  <si>
+    <t>OPO/LC team</t>
+  </si>
+  <si>
+    <t>OPO4</t>
   </si>
 </sst>
 </file>
@@ -1039,19 +1171,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C26"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.75" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>18</v>
       </c>
@@ -1061,8 +1194,11 @@
       <c r="C1" s="11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -1070,10 +1206,13 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1081,10 +1220,13 @@
         <v>32</v>
       </c>
       <c r="C3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -1092,10 +1234,13 @@
         <v>32</v>
       </c>
       <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -1103,10 +1248,13 @@
         <v>32</v>
       </c>
       <c r="C5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -1114,10 +1262,13 @@
         <v>32</v>
       </c>
       <c r="C6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -1125,10 +1276,13 @@
         <v>32</v>
       </c>
       <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -1136,10 +1290,13 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -1147,10 +1304,13 @@
         <v>34</v>
       </c>
       <c r="C9" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -1158,10 +1318,13 @@
         <v>35</v>
       </c>
       <c r="C10" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -1169,158 +1332,323 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>80</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>84</v>
+      </c>
+      <c r="C14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>85</v>
       </c>
-      <c r="C14" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>86</v>
-      </c>
       <c r="B15" t="s">
-        <v>87</v>
+        <v>162</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>94</v>
+        <v>160</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C18" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>106</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
         <v>0</v>
       </c>
       <c r="C20" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>118</v>
+        <v>175</v>
       </c>
       <c r="B21" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C21" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="B22" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="C22" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="B24" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="C24" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="B25" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="C25" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C26" t="s">
-        <v>141</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>150</v>
+      </c>
+      <c r="B27" t="s">
+        <v>151</v>
+      </c>
+      <c r="C27" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>153</v>
+      </c>
+      <c r="C28" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>154</v>
+      </c>
+      <c r="B29" t="s">
+        <v>155</v>
+      </c>
+      <c r="C29" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>158</v>
+      </c>
+      <c r="B30" t="s">
+        <v>118</v>
+      </c>
+      <c r="C30" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>166</v>
+      </c>
+      <c r="B32" t="s">
+        <v>167</v>
+      </c>
+      <c r="C32" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>169</v>
+      </c>
+      <c r="B33" t="s">
+        <v>170</v>
+      </c>
+      <c r="C33" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>172</v>
+      </c>
+      <c r="B34" t="s">
+        <v>173</v>
+      </c>
+      <c r="C34" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>176</v>
+      </c>
+      <c r="B35" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>178</v>
+      </c>
+      <c r="B36" t="s">
+        <v>118</v>
+      </c>
+      <c r="C36" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>180</v>
+      </c>
+      <c r="B37" t="s">
+        <v>118</v>
+      </c>
+      <c r="C37" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>183</v>
+      </c>
+      <c r="B38" t="s">
+        <v>184</v>
+      </c>
+      <c r="C38" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>185</v>
+      </c>
+      <c r="B39" t="s">
+        <v>186</v>
+      </c>
+      <c r="C39" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>188</v>
+      </c>
+      <c r="B40" t="s">
+        <v>189</v>
+      </c>
+      <c r="C40" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>191</v>
+      </c>
+      <c r="B41" t="s">
+        <v>192</v>
+      </c>
+      <c r="C41" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -1333,7 +1661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AY12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AX11" sqref="AX11"/>
     </sheetView>
   </sheetViews>
@@ -1465,82 +1793,82 @@
         <v>78</v>
       </c>
       <c r="Z1" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA1" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="AA1" s="13" t="s">
-        <v>83</v>
-      </c>
       <c r="AB1" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC1" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD1" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="AE1" s="13" t="s">
         <v>89</v>
       </c>
-      <c r="AC1" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="AD1" s="13" t="s">
-        <v>91</v>
-      </c>
-      <c r="AE1" s="13" t="s">
-        <v>92</v>
-      </c>
       <c r="AF1" s="13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="AG1" s="13" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="AH1" s="13" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="AI1" s="13" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="AJ1" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="AK1" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="AL1" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="AM1" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="AK1" s="13" t="s">
-        <v>111</v>
-      </c>
-      <c r="AL1" s="13" t="s">
-        <v>114</v>
-      </c>
-      <c r="AM1" s="13" t="s">
+      <c r="AN1" s="13" t="s">
         <v>115</v>
       </c>
-      <c r="AN1" s="13" t="s">
+      <c r="AO1" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="AP1" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="AO1" s="13" t="s">
-        <v>122</v>
-      </c>
-      <c r="AP1" s="13" t="s">
+      <c r="AR1" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="AS1" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="AQ1" s="13" t="s">
-        <v>127</v>
-      </c>
-      <c r="AR1" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="AS1" s="13" t="s">
-        <v>132</v>
-      </c>
       <c r="AT1" s="13" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="AU1" s="13" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="AV1" s="13" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="AW1" s="13" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="AX1" s="13" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="AY1" s="13" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
@@ -1656,13 +1984,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F5">
         <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -1672,13 +2000,13 @@
         <v>3</v>
       </c>
       <c r="M5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="X5" s="17">
         <v>4</v>
       </c>
       <c r="Y5" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="AN5" s="17">
         <v>4</v>
@@ -1846,7 +2174,7 @@
         <v>5</v>
       </c>
       <c r="AU11" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="AV11" s="17">
         <v>4</v>
@@ -1858,7 +2186,7 @@
         <v>2</v>
       </c>
       <c r="AY11" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.25">
@@ -1871,7 +2199,7 @@
         <v>2</v>
       </c>
       <c r="Q12" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
@@ -1879,25 +2207,25 @@
         <v>3</v>
       </c>
       <c r="AE12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AH12">
         <v>3</v>
       </c>
       <c r="AI12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AJ12">
         <v>3</v>
       </c>
       <c r="AK12" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="AL12">
         <v>3</v>
       </c>
       <c r="AM12" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New names from d3
</commit_message>
<xml_diff>
--- a/heatmaps/R-scr/HM-MS2.xlsx
+++ b/heatmaps/R-scr/HM-MS2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="206">
   <si>
     <t>PgM</t>
   </si>
@@ -523,9 +523,6 @@
     <t>TC1</t>
   </si>
   <si>
-    <t>CCB-A</t>
-  </si>
-  <si>
     <t>CCB-adm.</t>
   </si>
   <si>
@@ -620,6 +617,45 @@
   </si>
   <si>
     <t>OPO4</t>
+  </si>
+  <si>
+    <t>Lena Doverfors</t>
+  </si>
+  <si>
+    <t>CCB-admin</t>
+  </si>
+  <si>
+    <t>CCB-A1</t>
+  </si>
+  <si>
+    <t>CCB-A2</t>
+  </si>
+  <si>
+    <t>Ulf Olsson</t>
+  </si>
+  <si>
+    <t>CPI writer</t>
+  </si>
+  <si>
+    <t>CPIW1</t>
+  </si>
+  <si>
+    <t>Fredrik Svanfeldt</t>
+  </si>
+  <si>
+    <t>Department manager</t>
+  </si>
+  <si>
+    <t>DM3</t>
+  </si>
+  <si>
+    <t>Sven-Eric Ericson</t>
+  </si>
+  <si>
+    <t>Dsgnr8</t>
+  </si>
+  <si>
+    <t>SM4</t>
   </si>
 </sst>
 </file>
@@ -1171,10 +1207,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1362,10 +1398,10 @@
         <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C15" t="s">
-        <v>161</v>
+        <v>195</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1425,7 +1461,7 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B21" t="s">
         <v>113</v>
@@ -1532,123 +1568,175 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>162</v>
+      </c>
+      <c r="B31" t="s">
         <v>163</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>164</v>
-      </c>
-      <c r="C31" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>165</v>
+      </c>
+      <c r="B32" t="s">
         <v>166</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>167</v>
-      </c>
-      <c r="C32" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>168</v>
+      </c>
+      <c r="B33" t="s">
         <v>169</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>170</v>
-      </c>
-      <c r="C33" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>171</v>
+      </c>
+      <c r="B34" t="s">
         <v>172</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>173</v>
-      </c>
-      <c r="C34" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B35" t="s">
         <v>118</v>
       </c>
       <c r="C35" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B36" t="s">
         <v>118</v>
       </c>
       <c r="C36" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B37" t="s">
         <v>118</v>
       </c>
       <c r="C37" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>182</v>
+      </c>
+      <c r="B38" t="s">
         <v>183</v>
       </c>
-      <c r="B38" t="s">
-        <v>184</v>
-      </c>
       <c r="C38" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>184</v>
+      </c>
+      <c r="B39" t="s">
         <v>185</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>186</v>
-      </c>
-      <c r="C39" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40" t="s">
         <v>188</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>189</v>
-      </c>
-      <c r="C40" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>190</v>
+      </c>
+      <c r="B41" t="s">
         <v>191</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>192</v>
       </c>
-      <c r="C41" t="s">
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>193</v>
+      </c>
+      <c r="B42" t="s">
+        <v>194</v>
+      </c>
+      <c r="C42" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>197</v>
+      </c>
+      <c r="B43" t="s">
+        <v>198</v>
+      </c>
+      <c r="C43" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B44" t="s">
+        <v>188</v>
+      </c>
+      <c r="C44" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>200</v>
+      </c>
+      <c r="B45" t="s">
+        <v>201</v>
+      </c>
+      <c r="C45" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>203</v>
+      </c>
+      <c r="B46" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" t="s">
+        <v>204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Includes new names and codes
</commit_message>
<xml_diff>
--- a/heatmaps/R-scr/HM-MS2.xlsx
+++ b/heatmaps/R-scr/HM-MS2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="221">
   <si>
     <t>PgM</t>
   </si>
@@ -394,9 +394,6 @@
     <t>Designer</t>
   </si>
   <si>
-    <t>O7</t>
-  </si>
-  <si>
     <t>O7-I</t>
   </si>
   <si>
@@ -667,13 +664,43 @@
     <t>Section Manager (other org)</t>
   </si>
   <si>
-    <t>Sexction Manager (same org)</t>
-  </si>
-  <si>
     <t>Proj. Manager RBS Sys</t>
   </si>
   <si>
     <t>Jun Johansson</t>
+  </si>
+  <si>
+    <t>Section Manager (same org)</t>
+  </si>
+  <si>
+    <t>SM5</t>
+  </si>
+  <si>
+    <t>Eva Telandersson</t>
+  </si>
+  <si>
+    <t>TR-admin</t>
+  </si>
+  <si>
+    <t>TR-A1</t>
+  </si>
+  <si>
+    <t>Anna Ekedahl</t>
+  </si>
+  <si>
+    <t>CPI project lead</t>
+  </si>
+  <si>
+    <t>CPIPjL1</t>
+  </si>
+  <si>
+    <t>Johan Zhao</t>
+  </si>
+  <si>
+    <t>CPI</t>
+  </si>
+  <si>
+    <t>CPI1</t>
   </si>
 </sst>
 </file>
@@ -1225,10 +1252,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D47"/>
+  <dimension ref="A1:D50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1249,7 +1276,7 @@
         <v>20</v>
       </c>
       <c r="D1" s="11" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1260,7 +1287,7 @@
         <v>31</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D2" t="s">
         <v>37</v>
@@ -1344,7 +1371,7 @@
         <v>33</v>
       </c>
       <c r="C8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D8" t="s">
         <v>43</v>
@@ -1386,7 +1413,7 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D11" t="s">
         <v>46</v>
@@ -1400,7 +1427,7 @@
         <v>91</v>
       </c>
       <c r="C13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1408,7 +1435,7 @@
         <v>84</v>
       </c>
       <c r="B14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C14" t="s">
         <v>83</v>
@@ -1419,21 +1446,21 @@
         <v>85</v>
       </c>
       <c r="B15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C15" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B16" t="s">
         <v>90</v>
       </c>
       <c r="C16" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1466,7 +1493,7 @@
         <v>101</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1482,10 +1509,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C21" t="s">
         <v>113</v>
@@ -1499,282 +1526,315 @@
         <v>117</v>
       </c>
       <c r="C22" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B23" t="s">
         <v>34</v>
       </c>
       <c r="C23" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>125</v>
+      </c>
+      <c r="B24" t="s">
         <v>126</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>127</v>
-      </c>
-      <c r="C24" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>128</v>
+      </c>
+      <c r="B25" t="s">
         <v>129</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>130</v>
-      </c>
-      <c r="C25" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>131</v>
+      </c>
+      <c r="B26" t="s">
         <v>132</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>133</v>
-      </c>
-      <c r="C26" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>148</v>
+      </c>
+      <c r="B27" t="s">
         <v>149</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>150</v>
-      </c>
-      <c r="C27" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B28" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C28" t="s">
-        <v>118</v>
+        <v>211</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>152</v>
+      </c>
+      <c r="B29" t="s">
         <v>153</v>
       </c>
-      <c r="B29" t="s">
-        <v>154</v>
-      </c>
       <c r="C29" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B30" t="s">
         <v>117</v>
       </c>
       <c r="C30" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>160</v>
+      </c>
+      <c r="B31" t="s">
         <v>161</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>162</v>
-      </c>
-      <c r="C31" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B32" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>164</v>
+      </c>
+      <c r="B33" t="s">
         <v>165</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>166</v>
-      </c>
-      <c r="C33" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>167</v>
+      </c>
+      <c r="B34" t="s">
         <v>168</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>169</v>
-      </c>
-      <c r="C34" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B35" t="s">
         <v>117</v>
       </c>
       <c r="C35" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B36" t="s">
         <v>117</v>
       </c>
       <c r="C36" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B37" t="s">
         <v>117</v>
       </c>
       <c r="C37" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>178</v>
+      </c>
+      <c r="B38" t="s">
         <v>179</v>
       </c>
-      <c r="B38" t="s">
-        <v>180</v>
-      </c>
       <c r="C38" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>180</v>
+      </c>
+      <c r="B39" t="s">
         <v>181</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>182</v>
-      </c>
-      <c r="C39" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>183</v>
+      </c>
+      <c r="B40" t="s">
         <v>184</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>185</v>
-      </c>
-      <c r="C40" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>186</v>
+      </c>
+      <c r="B41" t="s">
         <v>187</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>188</v>
-      </c>
-      <c r="C41" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>189</v>
+      </c>
+      <c r="B42" t="s">
         <v>190</v>
       </c>
-      <c r="B42" t="s">
-        <v>191</v>
-      </c>
       <c r="C42" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
+        <v>193</v>
+      </c>
+      <c r="B43" t="s">
         <v>194</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>195</v>
-      </c>
-      <c r="C43" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B44" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C44" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>196</v>
+      </c>
+      <c r="B45" t="s">
         <v>197</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>198</v>
-      </c>
-      <c r="C45" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B46" t="s">
         <v>117</v>
       </c>
       <c r="C46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
+        <v>202</v>
+      </c>
+      <c r="B47" t="s">
         <v>203</v>
       </c>
-      <c r="B47" t="s">
+      <c r="C47" t="s">
         <v>204</v>
       </c>
-      <c r="C47" t="s">
-        <v>205</v>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>212</v>
+      </c>
+      <c r="B48" t="s">
+        <v>213</v>
+      </c>
+      <c r="C48" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>215</v>
+      </c>
+      <c r="B49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C49" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>218</v>
+      </c>
+      <c r="B50" t="s">
+        <v>219</v>
+      </c>
+      <c r="C50" t="s">
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -1967,34 +2027,34 @@
         <v>115</v>
       </c>
       <c r="AP1" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="AQ1" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="AQ1" s="13" t="s">
-        <v>120</v>
-      </c>
       <c r="AR1" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="AS1" s="13" t="s">
         <v>124</v>
       </c>
-      <c r="AS1" s="13" t="s">
-        <v>125</v>
-      </c>
       <c r="AT1" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="AU1" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="AU1" s="13" t="s">
+      <c r="AV1" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="AV1" s="13" t="s">
+      <c r="AW1" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="AW1" s="13" t="s">
+      <c r="AX1" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="AX1" s="13" t="s">
+      <c r="AY1" s="13" t="s">
         <v>139</v>
-      </c>
-      <c r="AY1" s="13" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="2" spans="1:51" x14ac:dyDescent="0.25">
@@ -2300,7 +2360,7 @@
         <v>5</v>
       </c>
       <c r="AU11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="AV11" s="17">
         <v>4</v>
@@ -2312,7 +2372,7 @@
         <v>2</v>
       </c>
       <c r="AY11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="12" spans="1:51" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adds new codes for d5
</commit_message>
<xml_diff>
--- a/heatmaps/R-scr/HM-MS2.xlsx
+++ b/heatmaps/R-scr/HM-MS2.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="237">
   <si>
     <t>PgM</t>
   </si>
@@ -685,9 +685,6 @@
     <t>CPIPjL1</t>
   </si>
   <si>
-    <t>Johan Zhao</t>
-  </si>
-  <si>
     <t>CPI</t>
   </si>
   <si>
@@ -707,6 +704,51 @@
   </si>
   <si>
     <t>Main Technical Coordinator</t>
+  </si>
+  <si>
+    <t>Niclas Fremling</t>
+  </si>
+  <si>
+    <t>Dsgnr9</t>
+  </si>
+  <si>
+    <t>Mats Nyrenius</t>
+  </si>
+  <si>
+    <t>Dsgnr10</t>
+  </si>
+  <si>
+    <t>Gunnar Lindh</t>
+  </si>
+  <si>
+    <t>CPI-writer</t>
+  </si>
+  <si>
+    <t>CPIW2</t>
+  </si>
+  <si>
+    <t>Sari Eklund</t>
+  </si>
+  <si>
+    <t>CPIW3</t>
+  </si>
+  <si>
+    <t>Irina Romanova</t>
+  </si>
+  <si>
+    <t>RBS2</t>
+  </si>
+  <si>
+    <t>Juhan Zhao</t>
+  </si>
+  <si>
+    <t>Karin Åkesson</t>
+  </si>
+  <si>
+    <t>CIRV</t>
+  </si>
+  <si>
+    <t>Cirv1</t>
   </si>
 </sst>
 </file>
@@ -1258,10 +1300,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1285,7 +1327,7 @@
         <v>139</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1450,7 +1492,7 @@
         <v>203</v>
       </c>
       <c r="C14" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1469,7 +1511,7 @@
         <v>117</v>
       </c>
       <c r="B16" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C16" t="s">
         <v>155</v>
@@ -1527,10 +1569,10 @@
         <v>204</v>
       </c>
       <c r="C21" t="s">
+        <v>219</v>
+      </c>
+      <c r="D21" t="s">
         <v>220</v>
-      </c>
-      <c r="D21" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1843,13 +1885,79 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>233</v>
+      </c>
+      <c r="B50" t="s">
         <v>215</v>
       </c>
-      <c r="B50" t="s">
+      <c r="C50" t="s">
         <v>216</v>
       </c>
-      <c r="C50" t="s">
-        <v>217</v>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>222</v>
+      </c>
+      <c r="B51" t="s">
+        <v>114</v>
+      </c>
+      <c r="C51" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>224</v>
+      </c>
+      <c r="B52" t="s">
+        <v>114</v>
+      </c>
+      <c r="C52" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>226</v>
+      </c>
+      <c r="B53" t="s">
+        <v>227</v>
+      </c>
+      <c r="C53" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>229</v>
+      </c>
+      <c r="B54" t="s">
+        <v>227</v>
+      </c>
+      <c r="C54" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>231</v>
+      </c>
+      <c r="B55" t="s">
+        <v>162</v>
+      </c>
+      <c r="C55" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>234</v>
+      </c>
+      <c r="B56" t="s">
+        <v>235</v>
+      </c>
+      <c r="C56" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adds xls for r2 d2.
</commit_message>
<xml_diff>
--- a/heatmaps/R-scr/HM-MS2.xlsx
+++ b/heatmaps/R-scr/HM-MS2.xlsx
@@ -640,9 +640,6 @@
     <t>Mats Eriksson</t>
   </si>
   <si>
-    <t>Change Leader</t>
-  </si>
-  <si>
     <t>CL1</t>
   </si>
   <si>
@@ -670,18 +667,12 @@
     <t>Eva Telandersson</t>
   </si>
   <si>
-    <t>TR-admin</t>
-  </si>
-  <si>
     <t>TR-A1</t>
   </si>
   <si>
     <t>Anna Ekedahl</t>
   </si>
   <si>
-    <t>CPI project lead</t>
-  </si>
-  <si>
     <t>CPIPjL1</t>
   </si>
   <si>
@@ -721,9 +712,6 @@
     <t>Gunnar Lindh</t>
   </si>
   <si>
-    <t>CPI-writer</t>
-  </si>
-  <si>
     <t>CPIW2</t>
   </si>
   <si>
@@ -749,6 +737,18 @@
   </si>
   <si>
     <t>Cirv1</t>
+  </si>
+  <si>
+    <t>O-XFT</t>
+  </si>
+  <si>
+    <t>CL</t>
+  </si>
+  <si>
+    <t>TR</t>
+  </si>
+  <si>
+    <t>RBS</t>
   </si>
 </sst>
 </file>
@@ -1302,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C56" sqref="A48:C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1327,7 +1327,7 @@
         <v>139</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -1489,10 +1489,10 @@
         <v>83</v>
       </c>
       <c r="B14" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C14" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1511,7 +1511,7 @@
         <v>117</v>
       </c>
       <c r="B16" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C16" t="s">
         <v>155</v>
@@ -1566,13 +1566,13 @@
         <v>167</v>
       </c>
       <c r="B21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C21" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D21" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1646,10 +1646,10 @@
         <v>148</v>
       </c>
       <c r="B28" t="s">
+        <v>206</v>
+      </c>
+      <c r="C28" t="s">
         <v>207</v>
-      </c>
-      <c r="C28" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1687,10 +1687,10 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B32" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C32" t="s">
         <v>160</v>
@@ -1819,7 +1819,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B44" t="s">
         <v>181</v>
@@ -1844,7 +1844,7 @@
         <v>196</v>
       </c>
       <c r="B46" t="s">
-        <v>114</v>
+        <v>233</v>
       </c>
       <c r="C46" t="s">
         <v>197</v>
@@ -1855,109 +1855,109 @@
         <v>199</v>
       </c>
       <c r="B47" t="s">
+        <v>234</v>
+      </c>
+      <c r="C47" t="s">
         <v>200</v>
-      </c>
-      <c r="C47" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>208</v>
+      </c>
+      <c r="B48" t="s">
+        <v>235</v>
+      </c>
+      <c r="C48" t="s">
         <v>209</v>
-      </c>
-      <c r="B48" t="s">
-        <v>210</v>
-      </c>
-      <c r="C48" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>210</v>
+      </c>
+      <c r="B49" t="s">
         <v>212</v>
       </c>
-      <c r="B49" t="s">
-        <v>213</v>
-      </c>
       <c r="C49" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="B50" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C50" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B51" t="s">
-        <v>114</v>
+        <v>233</v>
       </c>
       <c r="C51" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B52" t="s">
-        <v>114</v>
+        <v>233</v>
       </c>
       <c r="C52" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B53" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="C53" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B54" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
       <c r="C54" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B55" t="s">
-        <v>162</v>
+        <v>236</v>
       </c>
       <c r="C55" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="B56" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C56" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>